<commit_message>
Some of the more intense PVRP formats need some algorithm tweaking but otherwise everything is working fine.
</commit_message>
<xml_diff>
--- a/data/TR/results/PVRP_Comparison_Results.xlsx
+++ b/data/TR/results/PVRP_Comparison_Results.xlsx
@@ -224,16 +224,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.71875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.2890625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.2890625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.04296875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.04296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.05859375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.1953125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.30859375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="17.09375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.86328125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.69921875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5859375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5859375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.265625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.5859375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.734375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.41796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -295,6 +295,12 @@
       <c r="H3" t="n">
         <v>531.02</v>
       </c>
+      <c r="J3" t="n">
+        <v>1057.8831787109375</v>
+      </c>
+      <c r="K3" t="n">
+        <v>101.65519990677421</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -321,6 +327,12 @@
       <c r="H4" t="n">
         <v>1324.74</v>
       </c>
+      <c r="J4" t="n">
+        <v>2329.040283203125</v>
+      </c>
+      <c r="K4" t="n">
+        <v>76.05964933841761</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -341,6 +353,12 @@
       <c r="H5" t="n">
         <v>537.37</v>
       </c>
+      <c r="J5" t="n">
+        <v>1036.7662353515625</v>
+      </c>
+      <c r="K5" t="n">
+        <v>97.62985805405307</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -364,6 +382,12 @@
       <c r="H6" t="n">
         <v>845.97</v>
       </c>
+      <c r="J6" t="n">
+        <v>1630.29736328125</v>
+      </c>
+      <c r="K6" t="n">
+        <v>95.18441722113474</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -391,10 +415,10 @@
         <v>2043.75</v>
       </c>
       <c r="J7" t="n">
-        <v>3628.48193359375</v>
+        <v>4118.6328125</v>
       </c>
       <c r="K7" t="n">
-        <v>78.9201097438227</v>
+        <v>103.08940441027815</v>
       </c>
     </row>
     <row r="8">
@@ -416,6 +440,12 @@
       <c r="H8" t="n">
         <v>840.1</v>
       </c>
+      <c r="J8" t="n">
+        <v>1630.29736328125</v>
+      </c>
+      <c r="K8" t="n">
+        <v>95.14002792282602</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -439,6 +469,12 @@
       <c r="H9" t="n">
         <v>829.65</v>
       </c>
+      <c r="J9" t="n">
+        <v>1740.581787109375</v>
+      </c>
+      <c r="K9" t="n">
+        <v>110.6884773899551</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -465,6 +501,12 @@
       <c r="H10" t="n">
         <v>2052.21</v>
       </c>
+      <c r="J10" t="n">
+        <v>4622.36572265625</v>
+      </c>
+      <c r="K10" t="n">
+        <v>127.23819397076173</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -485,6 +527,12 @@
       <c r="H11" t="n">
         <v>829.65</v>
       </c>
+      <c r="J11" t="n">
+        <v>1740.581787109375</v>
+      </c>
+      <c r="K11" t="n">
+        <v>110.6884773899551</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -511,6 +559,12 @@
       <c r="H12" t="n">
         <v>1621.21</v>
       </c>
+      <c r="J12" t="n">
+        <v>3843.853515625</v>
+      </c>
+      <c r="K12" t="n">
+        <v>141.22837338008725</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -537,6 +591,12 @@
       <c r="H13" t="n">
         <v>782.17</v>
       </c>
+      <c r="J13" t="n">
+        <v>1651.6834716796875</v>
+      </c>
+      <c r="K13" t="n">
+        <v>112.00979021894176</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -557,6 +617,12 @@
       <c r="H14" t="n">
         <v>1230.95</v>
       </c>
+      <c r="J14" t="n">
+        <v>2275.407958984375</v>
+      </c>
+      <c r="K14" t="n">
+        <v>90.27059228220011</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -574,6 +640,12 @@
       <c r="G15" t="n">
         <v>3538.0</v>
       </c>
+      <c r="J15" t="n">
+        <v>10404.5673828125</v>
+      </c>
+      <c r="K15" t="n">
+        <v>196.2896720833262</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -591,6 +663,12 @@
       <c r="H16" t="n">
         <v>954.81</v>
       </c>
+      <c r="J16" t="n">
+        <v>1344.745361328125</v>
+      </c>
+      <c r="K16" t="n">
+        <v>40.840527998337336</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -608,6 +686,12 @@
       <c r="H17" t="n">
         <v>1862.63</v>
       </c>
+      <c r="J17" t="n">
+        <v>2697.02294921875</v>
+      </c>
+      <c r="K17" t="n">
+        <v>44.7988268666783</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -625,6 +709,12 @@
       <c r="H18" t="n">
         <v>2875.24</v>
       </c>
+      <c r="J18" t="n">
+        <v>4076.252685546875</v>
+      </c>
+      <c r="K18" t="n">
+        <v>41.77283964756799</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -642,6 +732,12 @@
       <c r="H19" t="n">
         <v>1597.75</v>
       </c>
+      <c r="J19" t="n">
+        <v>2766.99072265625</v>
+      </c>
+      <c r="K19" t="n">
+        <v>73.18045518111407</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -659,6 +755,12 @@
       <c r="H20" t="n">
         <v>3157.0</v>
       </c>
+      <c r="J20" t="n">
+        <v>5614.75927734375</v>
+      </c>
+      <c r="K20" t="n">
+        <v>78.8316450778182</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -676,6 +778,12 @@
       <c r="H21" t="n">
         <v>4846.49</v>
       </c>
+      <c r="J21" t="n">
+        <v>8550.53125</v>
+      </c>
+      <c r="K21" t="n">
+        <v>76.87070520484698</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -693,6 +801,12 @@
       <c r="H22" t="n">
         <v>8412.02</v>
       </c>
+      <c r="J22" t="n">
+        <v>14552.2802734375</v>
+      </c>
+      <c r="K22" t="n">
+        <v>73.91639306639459</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -710,6 +824,12 @@
       <c r="H23" t="n">
         <v>2173.58</v>
       </c>
+      <c r="J23" t="n">
+        <v>4158.62353515625</v>
+      </c>
+      <c r="K23" t="n">
+        <v>91.58778109177834</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -727,6 +847,12 @@
       <c r="H24" t="n">
         <v>4330.59</v>
       </c>
+      <c r="J24" t="n">
+        <v>8446.65234375</v>
+      </c>
+      <c r="K24" t="n">
+        <v>101.4008832663718</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -744,6 +870,12 @@
       <c r="H25" t="n">
         <v>6813.45</v>
       </c>
+      <c r="J25" t="n">
+        <v>12944.6767578125</v>
+      </c>
+      <c r="K25" t="n">
+        <v>101.60818286159162</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -761,6 +893,12 @@
       <c r="H26" t="n">
         <v>3702.02</v>
       </c>
+      <c r="J26" t="n">
+        <v>6702.60400390625</v>
+      </c>
+      <c r="K26" t="n">
+        <v>81.76750402461991</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -778,6 +916,12 @@
       <c r="H27" t="n">
         <v>3781.38</v>
       </c>
+      <c r="J27" t="n">
+        <v>6702.60400390625</v>
+      </c>
+      <c r="K27" t="n">
+        <v>77.45135893216445</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -795,6 +939,12 @@
       <c r="H28" t="n">
         <v>3795.33</v>
       </c>
+      <c r="J28" t="n">
+        <v>6702.60400390625</v>
+      </c>
+      <c r="K28" t="n">
+        <v>76.60181496965342</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
@@ -812,6 +962,12 @@
       <c r="H29" t="n">
         <v>22561.33</v>
       </c>
+      <c r="J29" t="n">
+        <v>47038.265625</v>
+      </c>
+      <c r="K29" t="n">
+        <v>114.23877584714884</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
@@ -829,6 +985,12 @@
       <c r="H30" t="n">
         <v>22562.44</v>
       </c>
+      <c r="J30" t="n">
+        <v>47038.265625</v>
+      </c>
+      <c r="K30" t="n">
+        <v>110.88342802665193</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
@@ -846,6 +1008,12 @@
       <c r="H31" t="n">
         <v>23752.15</v>
       </c>
+      <c r="J31" t="n">
+        <v>47038.265625</v>
+      </c>
+      <c r="K31" t="n">
+        <v>107.76756747504953</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -863,6 +1031,12 @@
       <c r="H32" t="n">
         <v>76793.99</v>
       </c>
+      <c r="J32" t="n">
+        <v>179766.265625</v>
+      </c>
+      <c r="K32" t="n">
+        <v>141.41281418092385</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
@@ -880,6 +1054,12 @@
       <c r="H33" t="n">
         <v>77944.79</v>
       </c>
+      <c r="J33" t="n">
+        <v>179766.265625</v>
+      </c>
+      <c r="K33" t="n">
+        <v>134.8281933254738</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
@@ -897,6 +1077,12 @@
       <c r="H34" t="n">
         <v>81055.52</v>
       </c>
+      <c r="J34" t="n">
+        <v>179766.265625</v>
+      </c>
+      <c r="K34" t="n">
+        <v>130.254431020093</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
@@ -908,6 +1094,12 @@
       <c r="C35" t="n">
         <v>2209.02</v>
       </c>
+      <c r="J35" t="n">
+        <v>3269.283447265625</v>
+      </c>
+      <c r="K35" t="n">
+        <v>47.99700533565223</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
@@ -919,6 +1111,12 @@
       <c r="C36" t="n">
         <v>3774.09</v>
       </c>
+      <c r="J36" t="n">
+        <v>7132.0732421875</v>
+      </c>
+      <c r="K36" t="n">
+        <v>88.97464666151308</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
@@ -930,6 +1128,12 @@
       <c r="C37" t="n">
         <v>5175.15</v>
       </c>
+      <c r="J37" t="n">
+        <v>9942.7802734375</v>
+      </c>
+      <c r="K37" t="n">
+        <v>92.12545092292012</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
@@ -941,6 +1145,12 @@
       <c r="C38" t="n">
         <v>5914.93</v>
       </c>
+      <c r="J38" t="n">
+        <v>12157.337890625</v>
+      </c>
+      <c r="K38" t="n">
+        <v>105.53646265678543</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
@@ -952,6 +1162,12 @@
       <c r="C39" t="n">
         <v>6618.95</v>
       </c>
+      <c r="J39" t="n">
+        <v>14563.259765625</v>
+      </c>
+      <c r="K39" t="n">
+        <v>120.02371623331496</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
@@ -963,6 +1179,12 @@
       <c r="C40" t="n">
         <v>8258.08</v>
       </c>
+      <c r="J40" t="n">
+        <v>17321.375</v>
+      </c>
+      <c r="K40" t="n">
+        <v>109.75063210818979</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
@@ -974,6 +1196,12 @@
       <c r="C41" t="n">
         <v>4996.14</v>
       </c>
+      <c r="J41" t="n">
+        <v>8236.38671875</v>
+      </c>
+      <c r="K41" t="n">
+        <v>64.85500243688128</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
@@ -985,6 +1213,12 @@
       <c r="C42" t="n">
         <v>6989.81</v>
       </c>
+      <c r="J42" t="n">
+        <v>14926.22265625</v>
+      </c>
+      <c r="K42" t="n">
+        <v>113.54260925904995</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
@@ -996,6 +1230,12 @@
       <c r="C43" t="n">
         <v>10075.4</v>
       </c>
+      <c r="J43" t="n">
+        <v>22524.71875</v>
+      </c>
+      <c r="K43" t="n">
+        <v>123.56153353713006</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
@@ -1006,6 +1246,12 @@
       </c>
       <c r="C44" t="n">
         <v>12924.66</v>
+      </c>
+      <c r="J44" t="n">
+        <v>26379.75</v>
+      </c>
+      <c r="K44" t="n">
+        <v>104.10401511529122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
insertion algorithm is fully functional
</commit_message>
<xml_diff>
--- a/data/TR/results/PVRP_Comparison_Results.xlsx
+++ b/data/TR/results/PVRP_Comparison_Results.xlsx
@@ -44,10 +44,10 @@
     <t>ALP</t>
   </si>
   <si>
-    <t>CPSC_464</t>
-  </si>
-  <si>
-    <t>%_Worse</t>
+    <t>ZEUS</t>
+  </si>
+  <si>
+    <t>%Difference_Best</t>
   </si>
   <si>
     <t>p1</t>
@@ -224,16 +224,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.71875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.2890625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.2890625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.04296875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.04296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.05859375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.1953125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.30859375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.8984375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="15.8984375" collapsed="true"/>
+    <col min="1" max="1" width="22.71875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.2890625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.2890625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="7.04296875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="7.04296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="7.05859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -479,12 +475,6 @@
       <c r="H11" t="n">
         <v>829.65</v>
       </c>
-      <c r="J11" t="n">
-        <v>729.301025390625</v>
-      </c>
-      <c r="K11" t="n">
-        <v>-4.0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -537,12 +527,6 @@
       <c r="H13" t="n">
         <v>782.17</v>
       </c>
-      <c r="J13" t="n">
-        <v>1715.970703125</v>
-      </c>
-      <c r="K13" t="n">
-        <v>120.26168756257545</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -1002,6 +986,12 @@
       <c r="C43" t="n">
         <v>10075.4</v>
       </c>
+      <c r="J43" t="n">
+        <v>13729.7939453125</v>
+      </c>
+      <c r="K43" t="n">
+        <v>36.0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
@@ -1012,12 +1002,6 @@
       </c>
       <c r="C44" t="n">
         <v>12924.66</v>
-      </c>
-      <c r="J44" t="n">
-        <v>27938.33203125</v>
-      </c>
-      <c r="K44" t="n">
-        <v>116.16299408456393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started changing insertion algorithm to integrate better with core program for local optimization purposes
</commit_message>
<xml_diff>
--- a/data/TR/results/PVRP_Comparison_Results.xlsx
+++ b/data/TR/results/PVRP_Comparison_Results.xlsx
@@ -224,12 +224,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="9.2890625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.2890625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="7.04296875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="7.04296875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="7.05859375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.71875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.2890625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.2890625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.04296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.04296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.05859375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.1953125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.30859375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="5.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.87109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -317,6 +321,12 @@
       <c r="H4" t="n">
         <v>1324.74</v>
       </c>
+      <c r="J4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-100.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -985,12 +995,6 @@
       </c>
       <c r="C43" t="n">
         <v>10075.4</v>
-      </c>
-      <c r="J43" t="n">
-        <v>13729.7939453125</v>
-      </c>
-      <c r="K43" t="n">
-        <v>36.0</v>
       </c>
     </row>
     <row r="44">

</xml_diff>

<commit_message>
some long awaited push from decades ago
</commit_message>
<xml_diff>
--- a/data/TR/results/PVRP_Comparison_Results.xlsx
+++ b/data/TR/results/PVRP_Comparison_Results.xlsx
@@ -224,16 +224,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="9.2890625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.2890625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="7.04296875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="7.04296875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="7.05859375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="8.1953125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="9.30859375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="17.015625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="16.87109375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.69921875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5859375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5859375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.265625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.5859375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.69921875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.01171875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -295,6 +295,12 @@
       <c r="H3" t="n">
         <v>531.02</v>
       </c>
+      <c r="J3" t="n">
+        <v>722.67529296875</v>
+      </c>
+      <c r="K3" t="n">
+        <v>37.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -322,10 +328,10 @@
         <v>1324.74</v>
       </c>
       <c r="J4" t="n">
-        <v>1664.69970703125</v>
+        <v>1762.634521484375</v>
       </c>
       <c r="K4" t="n">
-        <v>25.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="5">
@@ -347,6 +353,12 @@
       <c r="H5" t="n">
         <v>537.37</v>
       </c>
+      <c r="J5" t="n">
+        <v>722.67529296875</v>
+      </c>
+      <c r="K5" t="n">
+        <v>37.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -370,6 +382,12 @@
       <c r="H6" t="n">
         <v>845.97</v>
       </c>
+      <c r="J6" t="n">
+        <v>1133.586669921875</v>
+      </c>
+      <c r="K6" t="n">
+        <v>35.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -396,6 +414,12 @@
       <c r="H7" t="n">
         <v>2043.75</v>
       </c>
+      <c r="J7" t="n">
+        <v>2895.0810546875</v>
+      </c>
+      <c r="K7" t="n">
+        <v>42.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -416,6 +440,12 @@
       <c r="H8" t="n">
         <v>840.1</v>
       </c>
+      <c r="J8" t="n">
+        <v>1133.586669921875</v>
+      </c>
+      <c r="K8" t="n">
+        <v>35.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -439,6 +469,12 @@
       <c r="H9" t="n">
         <v>829.65</v>
       </c>
+      <c r="J9" t="n">
+        <v>1149.4837646484375</v>
+      </c>
+      <c r="K9" t="n">
+        <v>39.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -465,6 +501,12 @@
       <c r="H10" t="n">
         <v>2052.21</v>
       </c>
+      <c r="J10" t="n">
+        <v>2680.65234375</v>
+      </c>
+      <c r="K10" t="n">
+        <v>31.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -485,6 +527,12 @@
       <c r="H11" t="n">
         <v>829.65</v>
       </c>
+      <c r="J11" t="n">
+        <v>1149.4837646484375</v>
+      </c>
+      <c r="K11" t="n">
+        <v>39.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -511,6 +559,12 @@
       <c r="H12" t="n">
         <v>1621.21</v>
       </c>
+      <c r="J12" t="n">
+        <v>2286.556396484375</v>
+      </c>
+      <c r="K12" t="n">
+        <v>43.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -537,6 +591,12 @@
       <c r="H13" t="n">
         <v>782.17</v>
       </c>
+      <c r="J13" t="n">
+        <v>1258.539794921875</v>
+      </c>
+      <c r="K13" t="n">
+        <v>61.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -557,6 +617,12 @@
       <c r="H14" t="n">
         <v>1230.95</v>
       </c>
+      <c r="J14" t="n">
+        <v>1764.2425537109375</v>
+      </c>
+      <c r="K14" t="n">
+        <v>47.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -574,6 +640,12 @@
       <c r="G15" t="n">
         <v>3538.0</v>
       </c>
+      <c r="J15" t="n">
+        <v>6050.01123046875</v>
+      </c>
+      <c r="K15" t="n">
+        <v>72.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -591,6 +663,12 @@
       <c r="H16" t="n">
         <v>954.81</v>
       </c>
+      <c r="J16" t="n">
+        <v>954.8070678710938</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -608,6 +686,12 @@
       <c r="H17" t="n">
         <v>1862.63</v>
       </c>
+      <c r="J17" t="n">
+        <v>1862.6314697265625</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -625,6 +709,12 @@
       <c r="H18" t="n">
         <v>2875.24</v>
       </c>
+      <c r="J18" t="n">
+        <v>2875.24072265625</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -642,6 +732,12 @@
       <c r="H19" t="n">
         <v>1597.75</v>
       </c>
+      <c r="J19" t="n">
+        <v>1703.8721923828125</v>
+      </c>
+      <c r="K19" t="n">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -659,6 +755,12 @@
       <c r="H20" t="n">
         <v>3157.0</v>
       </c>
+      <c r="J20" t="n">
+        <v>3215.44482421875</v>
+      </c>
+      <c r="K20" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -676,6 +778,12 @@
       <c r="H21" t="n">
         <v>4846.49</v>
       </c>
+      <c r="J21" t="n">
+        <v>4846.4912109375</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -693,6 +801,12 @@
       <c r="H22" t="n">
         <v>8412.02</v>
       </c>
+      <c r="J22" t="n">
+        <v>8367.3974609375</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -710,6 +824,12 @@
       <c r="H23" t="n">
         <v>2173.58</v>
       </c>
+      <c r="J23" t="n">
+        <v>2476.455322265625</v>
+      </c>
+      <c r="K23" t="n">
+        <v>14.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -727,6 +847,12 @@
       <c r="H24" t="n">
         <v>4330.59</v>
       </c>
+      <c r="J24" t="n">
+        <v>4583.64013671875</v>
+      </c>
+      <c r="K24" t="n">
+        <v>9.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -744,6 +870,12 @@
       <c r="H25" t="n">
         <v>6813.45</v>
       </c>
+      <c r="J25" t="n">
+        <v>6795.0166015625</v>
+      </c>
+      <c r="K25" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -761,6 +893,12 @@
       <c r="H26" t="n">
         <v>3702.02</v>
       </c>
+      <c r="J26" t="n">
+        <v>5045.349609375</v>
+      </c>
+      <c r="K26" t="n">
+        <v>36.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -778,6 +916,12 @@
       <c r="H27" t="n">
         <v>3781.38</v>
       </c>
+      <c r="J27" t="n">
+        <v>5045.349609375</v>
+      </c>
+      <c r="K27" t="n">
+        <v>33.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -795,6 +939,12 @@
       <c r="H28" t="n">
         <v>3795.33</v>
       </c>
+      <c r="J28" t="n">
+        <v>5040.25439453125</v>
+      </c>
+      <c r="K28" t="n">
+        <v>32.0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
@@ -812,6 +962,12 @@
       <c r="H29" t="n">
         <v>22561.33</v>
       </c>
+      <c r="J29" t="n">
+        <v>33524.46484375</v>
+      </c>
+      <c r="K29" t="n">
+        <v>52.0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
@@ -829,6 +985,12 @@
       <c r="H30" t="n">
         <v>22562.44</v>
       </c>
+      <c r="J30" t="n">
+        <v>33297.10546875</v>
+      </c>
+      <c r="K30" t="n">
+        <v>49.0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
@@ -846,6 +1008,12 @@
       <c r="H31" t="n">
         <v>23752.15</v>
       </c>
+      <c r="J31" t="n">
+        <v>33343.578125</v>
+      </c>
+      <c r="K31" t="n">
+        <v>47.0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -863,6 +1031,12 @@
       <c r="H32" t="n">
         <v>76793.99</v>
       </c>
+      <c r="J32" t="n">
+        <v>124680.8046875</v>
+      </c>
+      <c r="K32" t="n">
+        <v>67.0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
@@ -880,6 +1054,12 @@
       <c r="H33" t="n">
         <v>77944.79</v>
       </c>
+      <c r="J33" t="n">
+        <v>125849.21875</v>
+      </c>
+      <c r="K33" t="n">
+        <v>64.0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
@@ -897,6 +1077,12 @@
       <c r="H34" t="n">
         <v>81055.52</v>
       </c>
+      <c r="J34" t="n">
+        <v>124782.9140625</v>
+      </c>
+      <c r="K34" t="n">
+        <v>59.0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
@@ -908,6 +1094,12 @@
       <c r="C35" t="n">
         <v>2209.02</v>
       </c>
+      <c r="J35" t="n">
+        <v>2734.0546875</v>
+      </c>
+      <c r="K35" t="n">
+        <v>23.0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
@@ -919,6 +1111,12 @@
       <c r="C36" t="n">
         <v>3774.09</v>
       </c>
+      <c r="J36" t="n">
+        <v>5192.5439453125</v>
+      </c>
+      <c r="K36" t="n">
+        <v>37.0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
@@ -930,6 +1128,12 @@
       <c r="C37" t="n">
         <v>5175.15</v>
       </c>
+      <c r="J37" t="n">
+        <v>8074.99609375</v>
+      </c>
+      <c r="K37" t="n">
+        <v>56.0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
@@ -941,6 +1145,12 @@
       <c r="C38" t="n">
         <v>5914.93</v>
       </c>
+      <c r="J38" t="n">
+        <v>9463.0966796875</v>
+      </c>
+      <c r="K38" t="n">
+        <v>59.0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
@@ -963,6 +1173,12 @@
       <c r="C40" t="n">
         <v>8258.08</v>
       </c>
+      <c r="J40" t="n">
+        <v>13173.0625</v>
+      </c>
+      <c r="K40" t="n">
+        <v>59.0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
@@ -985,6 +1201,12 @@
       <c r="C42" t="n">
         <v>6989.81</v>
       </c>
+      <c r="J42" t="n">
+        <v>10987.5703125</v>
+      </c>
+      <c r="K42" t="n">
+        <v>57.0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
@@ -995,6 +1217,12 @@
       </c>
       <c r="C43" t="n">
         <v>10075.4</v>
+      </c>
+      <c r="J43" t="n">
+        <v>16791.888671875</v>
+      </c>
+      <c r="K43" t="n">
+        <v>66.0</v>
       </c>
     </row>
     <row r="44">

</xml_diff>